<commit_message>
Bat file Window function established
Final version of project, Commit changes
</commit_message>
<xml_diff>
--- a/API_stock_prices.xlsx
+++ b/API_stock_prices.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H50"/>
+  <dimension ref="A1:H64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,27 +476,27 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>BAJAJHIND.BO</t>
+          <t>BANKINDIA.NS</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>19.06999969482422</v>
+        <v>110.2200012207031</v>
       </c>
       <c r="D2" t="n">
-        <v>17.96999931335449</v>
+        <v>104.1999969482422</v>
       </c>
       <c r="E2" t="n">
-        <v>19.35000038146973</v>
+        <v>111.2200012207031</v>
       </c>
       <c r="F2" t="n">
-        <v>17.96999931335449</v>
+        <v>104.1999969482422</v>
       </c>
       <c r="G2" t="n">
-        <v>18.73999977111816</v>
+        <v>107.8600006103516</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>BAJAJHIND</t>
+          <t>BANKINDIA</t>
         </is>
       </c>
     </row>
@@ -506,27 +506,27 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>BANDHANBNK.BO</t>
+          <t>COCHINSHIP.NS</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>156.9499969482422</v>
+        <v>1484.599975585938</v>
       </c>
       <c r="D3" t="n">
-        <v>153.6000061035156</v>
+        <v>1426.199951171875</v>
       </c>
       <c r="E3" t="n">
-        <v>157.9499969482422</v>
+        <v>1492</v>
       </c>
       <c r="F3" t="n">
-        <v>153.0500030517578</v>
+        <v>1417.900024414062</v>
       </c>
       <c r="G3" t="n">
-        <v>157.3000030517578</v>
+        <v>1443.400024414062</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>BANDHANBNK</t>
+          <t>COCHINSHIP</t>
         </is>
       </c>
     </row>
@@ -536,27 +536,27 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>BANKBARODA.NS</t>
+          <t>EXCELINDUS.NS</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>220.0899963378906</v>
+        <v>1024</v>
       </c>
       <c r="D4" t="n">
-        <v>212.9900054931641</v>
+        <v>1004.5</v>
       </c>
       <c r="E4" t="n">
-        <v>220.5</v>
+        <v>1038</v>
       </c>
       <c r="F4" t="n">
-        <v>212.5500030517578</v>
+        <v>991.0999755859375</v>
       </c>
       <c r="G4" t="n">
-        <v>217.2700042724609</v>
+        <v>1046.400024414062</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>BANKBARODA</t>
+          <t>EXCELINDUS</t>
         </is>
       </c>
     </row>
@@ -566,27 +566,27 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>BHEL.BO</t>
+          <t>EXIDEIND.NS</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>216.75</v>
+        <v>360.9500122070312</v>
       </c>
       <c r="D5" t="n">
-        <v>210.3999938964844</v>
+        <v>350.5</v>
       </c>
       <c r="E5" t="n">
-        <v>217.9499969482422</v>
+        <v>362.2000122070312</v>
       </c>
       <c r="F5" t="n">
-        <v>210.3999938964844</v>
+        <v>350.5</v>
       </c>
       <c r="G5" t="n">
-        <v>217.3500061035156</v>
+        <v>360.8500061035156</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>BHEL</t>
+          <t>EXIDEIND</t>
         </is>
       </c>
     </row>
@@ -596,27 +596,27 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>BIGBLOC.NS</t>
+          <t>HAPPSTMNDS.NS</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>62.11000061035156</v>
+        <v>577.5</v>
       </c>
       <c r="D6" t="n">
-        <v>60.16999816894531</v>
+        <v>563.2999877929688</v>
       </c>
       <c r="E6" t="n">
-        <v>62.84999847412109</v>
+        <v>580</v>
       </c>
       <c r="F6" t="n">
-        <v>59.95999908447266</v>
+        <v>560.5499877929688</v>
       </c>
       <c r="G6" t="n">
-        <v>62.84999847412109</v>
+        <v>585.0499877929688</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>BIGBLOC</t>
+          <t>HAPPSTMNDS</t>
         </is>
       </c>
     </row>
@@ -626,27 +626,27 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>CANBK.BO</t>
+          <t>HINDUNILVR.BO</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>97.65000152587891</v>
+        <v>2333.949951171875</v>
       </c>
       <c r="D7" t="n">
-        <v>93.66000366210938</v>
+        <v>2324.10009765625</v>
       </c>
       <c r="E7" t="n">
-        <v>98.40000152587891</v>
+        <v>2340</v>
       </c>
       <c r="F7" t="n">
-        <v>93.66000366210938</v>
+        <v>2302</v>
       </c>
       <c r="G7" t="n">
-        <v>95.37999725341797</v>
+        <v>2355.25</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>CANBK</t>
+          <t>HINDUNILVR</t>
         </is>
       </c>
     </row>
@@ -656,27 +656,27 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>COCHINSHIP.BO</t>
+          <t>IDFCFIRSTB.BO</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>1484.400024414062</v>
+        <v>66.20999908447266</v>
       </c>
       <c r="D8" t="n">
-        <v>1435</v>
+        <v>64.84999847412109</v>
       </c>
       <c r="E8" t="n">
-        <v>1491.699951171875</v>
+        <v>66.90000152587891</v>
       </c>
       <c r="F8" t="n">
-        <v>1415.449951171875</v>
+        <v>64.84999847412109</v>
       </c>
       <c r="G8" t="n">
-        <v>1444.099975585938</v>
+        <v>66.44999694824219</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>COCHINSHIP</t>
+          <t>IDFCFIRSTB</t>
         </is>
       </c>
     </row>
@@ -686,27 +686,27 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>DELTACORP.BO</t>
+          <t>KPIGREEN.BO</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>84.80000305175781</v>
+        <v>348.6000061035156</v>
       </c>
       <c r="D9" t="n">
-        <v>81.61000061035156</v>
+        <v>335.6000061035156</v>
       </c>
       <c r="E9" t="n">
-        <v>87.75</v>
+        <v>351.75</v>
       </c>
       <c r="F9" t="n">
-        <v>81.61000061035156</v>
+        <v>335.5499877929688</v>
       </c>
       <c r="G9" t="n">
-        <v>88.54000091552734</v>
+        <v>358.8999938964844</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>DELTACORP</t>
+          <t>KPIGREEN</t>
         </is>
       </c>
     </row>
@@ -716,27 +716,27 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>EMBDL.NS</t>
+          <t>MAHABANK.BO</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>91.29000091552734</v>
+        <v>48.34999847412109</v>
       </c>
       <c r="D10" t="n">
-        <v>90</v>
+        <v>47.13999938964844</v>
       </c>
       <c r="E10" t="n">
-        <v>92.08999633789062</v>
+        <v>49.13000106811523</v>
       </c>
       <c r="F10" t="n">
-        <v>89.22000122070312</v>
+        <v>47.13999938964844</v>
       </c>
       <c r="G10" t="n">
-        <v>91.55999755859375</v>
+        <v>48.91999816894531</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>EMBDL</t>
+          <t>MAHABANK</t>
         </is>
       </c>
     </row>
@@ -746,27 +746,27 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>EXIDEIND.NS</t>
+          <t>RELIANCE.BO</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>360.9500122070312</v>
+        <v>1377.75</v>
       </c>
       <c r="D11" t="n">
-        <v>350.5</v>
+        <v>1372.050048828125</v>
       </c>
       <c r="E11" t="n">
-        <v>362.2000122070312</v>
+        <v>1395</v>
       </c>
       <c r="F11" t="n">
-        <v>350.5</v>
+        <v>1372.050048828125</v>
       </c>
       <c r="G11" t="n">
-        <v>360.8500061035156</v>
+        <v>1404.849975585938</v>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>EXIDEIND</t>
+          <t>RELIANCE</t>
         </is>
       </c>
     </row>
@@ -776,27 +776,27 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>GLENMARK.NS</t>
+          <t>SAIL.NS</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>1398.199951171875</v>
+        <v>109.0100021362305</v>
       </c>
       <c r="D12" t="n">
-        <v>1395</v>
+        <v>107</v>
       </c>
       <c r="E12" t="n">
-        <v>1414.199951171875</v>
+        <v>109.3199996948242</v>
       </c>
       <c r="F12" t="n">
-        <v>1382.900024414062</v>
+        <v>106.25</v>
       </c>
       <c r="G12" t="n">
-        <v>1418.900024414062</v>
+        <v>109.2399978637695</v>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>GLENMARK</t>
+          <t>SAIL</t>
         </is>
       </c>
     </row>
@@ -806,27 +806,27 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>HDFCBANK.NS</t>
+          <t>SOUTHBANK.BO</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>1889.699951171875</v>
+        <v>24.34000015258789</v>
       </c>
       <c r="D13" t="n">
-        <v>1910.099975585938</v>
+        <v>23.79000091552734</v>
       </c>
       <c r="E13" t="n">
-        <v>1919</v>
+        <v>24.43000030517578</v>
       </c>
       <c r="F13" t="n">
-        <v>1886.800048828125</v>
+        <v>23.79000091552734</v>
       </c>
       <c r="G13" t="n">
-        <v>1928.5</v>
+        <v>24.20000076293945</v>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>HDFCBANK</t>
+          <t>SOUTHBANK</t>
         </is>
       </c>
     </row>
@@ -836,27 +836,27 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>ICICIBANK.NS</t>
+          <t>TATAMOTORS.BO</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>1388.900024414062</v>
+        <v>708.5</v>
       </c>
       <c r="D14" t="n">
-        <v>1415.199951171875</v>
+        <v>662.5999755859375</v>
       </c>
       <c r="E14" t="n">
-        <v>1419.900024414062</v>
+        <v>710.8499755859375</v>
       </c>
       <c r="F14" t="n">
-        <v>1387</v>
+        <v>662.5999755859375</v>
       </c>
       <c r="G14" t="n">
-        <v>1435.5</v>
+        <v>681.9000244140625</v>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>ICICIBANK</t>
+          <t>TATAMOTORS</t>
         </is>
       </c>
     </row>
@@ -866,27 +866,27 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>IDBI.NS</t>
+          <t>TCS.BO</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>76.30000305175781</v>
+        <v>3442.199951171875</v>
       </c>
       <c r="D15" t="n">
-        <v>75.5</v>
+        <v>3380</v>
       </c>
       <c r="E15" t="n">
-        <v>76.66999816894531</v>
+        <v>3445.14990234375</v>
       </c>
       <c r="F15" t="n">
-        <v>75</v>
+        <v>3380</v>
       </c>
       <c r="G15" t="n">
-        <v>76.87000274658203</v>
+        <v>3447.449951171875</v>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>IDBI</t>
+          <t>TCS</t>
         </is>
       </c>
     </row>
@@ -896,27 +896,27 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>IDEA.BO</t>
+          <t>BAJAJHIND.BO</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>6.710000038146973</v>
+        <v>19.06999969482422</v>
       </c>
       <c r="D16" t="n">
-        <v>6.519999980926514</v>
+        <v>17.96999931335449</v>
       </c>
       <c r="E16" t="n">
-        <v>6.75</v>
+        <v>19.35000038146973</v>
       </c>
       <c r="F16" t="n">
-        <v>6.460000038146973</v>
+        <v>17.96999931335449</v>
       </c>
       <c r="G16" t="n">
-        <v>6.690000057220459</v>
+        <v>18.73999977111816</v>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>IDEA</t>
+          <t>BAJAJHIND</t>
         </is>
       </c>
     </row>
@@ -926,27 +926,27 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>IDFCFIRSTB.BO</t>
+          <t>BANDHANBNK.BO</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>66.20999908447266</v>
+        <v>156.9499969482422</v>
       </c>
       <c r="D17" t="n">
-        <v>64.84999847412109</v>
+        <v>153.6000061035156</v>
       </c>
       <c r="E17" t="n">
-        <v>66.90000152587891</v>
+        <v>157.9499969482422</v>
       </c>
       <c r="F17" t="n">
-        <v>64.84999847412109</v>
+        <v>153.0500030517578</v>
       </c>
       <c r="G17" t="n">
-        <v>66.44999694824219</v>
+        <v>157.3000030517578</v>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>IDFCFIRSTB</t>
+          <t>BANDHANBNK</t>
         </is>
       </c>
     </row>
@@ -956,27 +956,27 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>IEX.NS</t>
+          <t>BANKBARODA.NS</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>189.3800048828125</v>
+        <v>220.0899963378906</v>
       </c>
       <c r="D18" t="n">
-        <v>182</v>
+        <v>212.9900054931641</v>
       </c>
       <c r="E18" t="n">
-        <v>190.0500030517578</v>
+        <v>220.5</v>
       </c>
       <c r="F18" t="n">
-        <v>182</v>
+        <v>212.5500030517578</v>
       </c>
       <c r="G18" t="n">
-        <v>189.8999938964844</v>
+        <v>217.2700042724609</v>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>IEX</t>
+          <t>BANKBARODA</t>
         </is>
       </c>
     </row>
@@ -986,27 +986,27 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>ITC.NS</t>
+          <t>BHEL.BO</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>423.5499877929688</v>
+        <v>216.75</v>
       </c>
       <c r="D19" t="n">
-        <v>425.9500122070312</v>
+        <v>210.3999938964844</v>
       </c>
       <c r="E19" t="n">
-        <v>429.1499938964844</v>
+        <v>217.9499969482422</v>
       </c>
       <c r="F19" t="n">
-        <v>423</v>
+        <v>210.3999938964844</v>
       </c>
       <c r="G19" t="n">
-        <v>430.6000061035156</v>
+        <v>217.3500061035156</v>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>ITC</t>
+          <t>BHEL</t>
         </is>
       </c>
     </row>
@@ -1016,27 +1016,27 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>JPPOWER.BO</t>
+          <t>BIGBLOC.NS</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>13.27999973297119</v>
+        <v>62.11000061035156</v>
       </c>
       <c r="D20" t="n">
-        <v>12.60999965667725</v>
+        <v>60.16999816894531</v>
       </c>
       <c r="E20" t="n">
-        <v>13.39999961853027</v>
+        <v>62.84999847412109</v>
       </c>
       <c r="F20" t="n">
-        <v>12.60999965667725</v>
+        <v>59.95999908447266</v>
       </c>
       <c r="G20" t="n">
-        <v>13.26000022888184</v>
+        <v>62.84999847412109</v>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>JPPOWER</t>
+          <t>BIGBLOC</t>
         </is>
       </c>
     </row>
@@ -1046,27 +1046,27 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>KALAMANDIR.NS</t>
+          <t>CANBK.BO</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>113.5100021362305</v>
+        <v>97.65000152587891</v>
       </c>
       <c r="D21" t="n">
-        <v>113</v>
+        <v>93.66000366210938</v>
       </c>
       <c r="E21" t="n">
-        <v>114.8899993896484</v>
+        <v>98.40000152587891</v>
       </c>
       <c r="F21" t="n">
-        <v>113</v>
+        <v>93.66000366210938</v>
       </c>
       <c r="G21" t="n">
-        <v>114.7799987792969</v>
+        <v>95.37999725341797</v>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>KALAMANDIR</t>
+          <t>CANBK</t>
         </is>
       </c>
     </row>
@@ -1076,27 +1076,27 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>KPIGREEN.NS</t>
+          <t>COCHINSHIP.BO</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>348.3500061035156</v>
+        <v>1484.400024414062</v>
       </c>
       <c r="D22" t="n">
-        <v>336</v>
+        <v>1435</v>
       </c>
       <c r="E22" t="n">
-        <v>352</v>
+        <v>1491.699951171875</v>
       </c>
       <c r="F22" t="n">
-        <v>336</v>
+        <v>1415.449951171875</v>
       </c>
       <c r="G22" t="n">
-        <v>359.25</v>
+        <v>1444.099975585938</v>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>KPIGREEN</t>
+          <t>COCHINSHIP</t>
         </is>
       </c>
     </row>
@@ -1106,27 +1106,27 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>LTF.NS</t>
+          <t>DELTACORP.BO</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>161.5299987792969</v>
+        <v>84.80000305175781</v>
       </c>
       <c r="D23" t="n">
-        <v>159.7400054931641</v>
+        <v>81.61000061035156</v>
       </c>
       <c r="E23" t="n">
-        <v>164.1699981689453</v>
+        <v>87.75</v>
       </c>
       <c r="F23" t="n">
-        <v>159.6600036621094</v>
+        <v>81.61000061035156</v>
       </c>
       <c r="G23" t="n">
-        <v>163.5299987792969</v>
+        <v>88.54000091552734</v>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>LTF</t>
+          <t>DELTACORP</t>
         </is>
       </c>
     </row>
@@ -1136,27 +1136,27 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>LAURUSLABS.NS</t>
+          <t>EMBDL.NS</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>588.7999877929688</v>
+        <v>91.29000091552734</v>
       </c>
       <c r="D24" t="n">
-        <v>578</v>
+        <v>90</v>
       </c>
       <c r="E24" t="n">
-        <v>590</v>
+        <v>92.08999633789062</v>
       </c>
       <c r="F24" t="n">
-        <v>572.25</v>
+        <v>89.22000122070312</v>
       </c>
       <c r="G24" t="n">
-        <v>585.9500122070312</v>
+        <v>91.55999755859375</v>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>LAURUSLABS</t>
+          <t>EMBDL</t>
         </is>
       </c>
     </row>
@@ -1166,27 +1166,27 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>NTPC.NS</t>
+          <t>EXIDEIND.NS</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>334.75</v>
+        <v>360.9500122070312</v>
       </c>
       <c r="D25" t="n">
-        <v>334.2000122070312</v>
+        <v>350.5</v>
       </c>
       <c r="E25" t="n">
-        <v>338.75</v>
+        <v>362.2000122070312</v>
       </c>
       <c r="F25" t="n">
-        <v>330.6000061035156</v>
+        <v>350.5</v>
       </c>
       <c r="G25" t="n">
-        <v>340</v>
+        <v>360.8500061035156</v>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>NTPC</t>
+          <t>EXIDEIND</t>
         </is>
       </c>
     </row>
@@ -1196,27 +1196,27 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>ONGC.NS</t>
+          <t>GLENMARK.NS</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>234.9600067138672</v>
+        <v>1398.199951171875</v>
       </c>
       <c r="D26" t="n">
-        <v>229.1000061035156</v>
+        <v>1395</v>
       </c>
       <c r="E26" t="n">
-        <v>235.3000030517578</v>
+        <v>1414.199951171875</v>
       </c>
       <c r="F26" t="n">
-        <v>228.4499969482422</v>
+        <v>1382.900024414062</v>
       </c>
       <c r="G26" t="n">
-        <v>233.2200012207031</v>
+        <v>1418.900024414062</v>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>ONGC</t>
+          <t>GLENMARK</t>
         </is>
       </c>
     </row>
@@ -1226,27 +1226,27 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>PNB.NS</t>
+          <t>HDFCBANK.NS</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>91.97000122070312</v>
+        <v>1889.699951171875</v>
       </c>
       <c r="D27" t="n">
-        <v>90</v>
+        <v>1910.099975585938</v>
       </c>
       <c r="E27" t="n">
-        <v>92.34999847412109</v>
+        <v>1919</v>
       </c>
       <c r="F27" t="n">
-        <v>89.44999694824219</v>
+        <v>1886.800048828125</v>
       </c>
       <c r="G27" t="n">
-        <v>91.36000061035156</v>
+        <v>1928.5</v>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>PNB</t>
+          <t>HDFCBANK</t>
         </is>
       </c>
     </row>
@@ -1256,27 +1256,27 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>PREMIERENE.NS</t>
+          <t>ICICIBANK.NS</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>945.6500244140625</v>
+        <v>1388.900024414062</v>
       </c>
       <c r="D28" t="n">
-        <v>922</v>
+        <v>1415.199951171875</v>
       </c>
       <c r="E28" t="n">
-        <v>954</v>
+        <v>1419.900024414062</v>
       </c>
       <c r="F28" t="n">
-        <v>917.0499877929688</v>
+        <v>1387</v>
       </c>
       <c r="G28" t="n">
-        <v>944.7000122070312</v>
+        <v>1435.5</v>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>PREMIERENE</t>
+          <t>ICICIBANK</t>
         </is>
       </c>
     </row>
@@ -1286,27 +1286,27 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>RPOWER.BO</t>
+          <t>IDBI.NS</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>38.65000152587891</v>
+        <v>76.30000305175781</v>
       </c>
       <c r="D29" t="n">
-        <v>37.13999938964844</v>
+        <v>75.5</v>
       </c>
       <c r="E29" t="n">
-        <v>38.84999847412109</v>
+        <v>76.66999816894531</v>
       </c>
       <c r="F29" t="n">
-        <v>37</v>
+        <v>75</v>
       </c>
       <c r="G29" t="n">
-        <v>38.29000091552734</v>
+        <v>76.87000274658203</v>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>RPOWER</t>
+          <t>IDBI</t>
         </is>
       </c>
     </row>
@@ -1316,27 +1316,27 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>SBIN.NS</t>
+          <t>IDEA.BO</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>779.25</v>
+        <v>6.710000038146973</v>
       </c>
       <c r="D30" t="n">
-        <v>756.5</v>
+        <v>6.519999980926514</v>
       </c>
       <c r="E30" t="n">
-        <v>781.7000122070312</v>
+        <v>6.75</v>
       </c>
       <c r="F30" t="n">
-        <v>755.5</v>
+        <v>6.460000038146973</v>
       </c>
       <c r="G30" t="n">
-        <v>769</v>
+        <v>6.690000057220459</v>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>SBIN</t>
+          <t>IDEA</t>
         </is>
       </c>
     </row>
@@ -1346,27 +1346,27 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>SUVEN.NS</t>
+          <t>IDFCFIRSTB.BO</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>142.4499969482422</v>
+        <v>66.20999908447266</v>
       </c>
       <c r="D31" t="n">
-        <v>136.9900054931641</v>
+        <v>64.84999847412109</v>
       </c>
       <c r="E31" t="n">
-        <v>144.0299987792969</v>
+        <v>66.90000152587891</v>
       </c>
       <c r="F31" t="n">
-        <v>131.9900054931641</v>
+        <v>64.84999847412109</v>
       </c>
       <c r="G31" t="n">
-        <v>137.8300018310547</v>
+        <v>66.44999694824219</v>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>SUVEN</t>
+          <t>IDFCFIRSTB</t>
         </is>
       </c>
     </row>
@@ -1376,27 +1376,27 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>TATAMOTORS.NS</t>
+          <t>IEX.NS</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>708.5</v>
+        <v>189.3800048828125</v>
       </c>
       <c r="D32" t="n">
-        <v>667.5</v>
+        <v>182</v>
       </c>
       <c r="E32" t="n">
-        <v>711</v>
+        <v>190.0500030517578</v>
       </c>
       <c r="F32" t="n">
-        <v>666</v>
+        <v>182</v>
       </c>
       <c r="G32" t="n">
-        <v>682.8499755859375</v>
+        <v>189.8999938964844</v>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>TATAMOTORS</t>
+          <t>IEX</t>
         </is>
       </c>
     </row>
@@ -1406,27 +1406,27 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>TECHM.NS</t>
+          <t>ITC.NS</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>1493.699951171875</v>
+        <v>423.5499877929688</v>
       </c>
       <c r="D33" t="n">
-        <v>1480</v>
+        <v>425.9500122070312</v>
       </c>
       <c r="E33" t="n">
-        <v>1501.300048828125</v>
+        <v>429.1499938964844</v>
       </c>
       <c r="F33" t="n">
-        <v>1478.099975585938</v>
+        <v>423</v>
       </c>
       <c r="G33" t="n">
-        <v>1502.800048828125</v>
+        <v>430.6000061035156</v>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>TECHM</t>
+          <t>ITC</t>
         </is>
       </c>
     </row>
@@ -1436,27 +1436,27 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>TFCILTD.BO</t>
+          <t>JPPOWER.BO</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>196.3000030517578</v>
+        <v>13.27999973297119</v>
       </c>
       <c r="D34" t="n">
-        <v>195</v>
+        <v>12.60999965667725</v>
       </c>
       <c r="E34" t="n">
-        <v>198.8500061035156</v>
+        <v>13.39999961853027</v>
       </c>
       <c r="F34" t="n">
-        <v>185</v>
+        <v>12.60999965667725</v>
       </c>
       <c r="G34" t="n">
-        <v>198.1999969482422</v>
+        <v>13.26000022888184</v>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>TFCILTD</t>
+          <t>JPPOWER</t>
         </is>
       </c>
     </row>
@@ -1466,27 +1466,27 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>UCOBANK.BO</t>
+          <t>KALAMANDIR.NS</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>29.59000015258789</v>
+        <v>113.5100021362305</v>
       </c>
       <c r="D35" t="n">
-        <v>29.36000061035156</v>
+        <v>113</v>
       </c>
       <c r="E35" t="n">
-        <v>29.89999961853027</v>
+        <v>114.8899993896484</v>
       </c>
       <c r="F35" t="n">
-        <v>29.04999923706055</v>
+        <v>113</v>
       </c>
       <c r="G35" t="n">
-        <v>29.98999786376953</v>
+        <v>114.7799987792969</v>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>UCOBANK</t>
+          <t>KALAMANDIR</t>
         </is>
       </c>
     </row>
@@ -1496,27 +1496,27 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>VAKRANGEE.NS</t>
+          <t>KPIGREEN.NS</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>8.840000152587891</v>
+        <v>348.3500061035156</v>
       </c>
       <c r="D36" t="n">
-        <v>9</v>
+        <v>336</v>
       </c>
       <c r="E36" t="n">
-        <v>9.180000305175781</v>
+        <v>352</v>
       </c>
       <c r="F36" t="n">
-        <v>8.819999694824219</v>
+        <v>336</v>
       </c>
       <c r="G36" t="n">
-        <v>9.229999542236328</v>
+        <v>359.25</v>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>VAKRANGEE</t>
+          <t>KPIGREEN</t>
         </is>
       </c>
     </row>
@@ -1526,27 +1526,27 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>VISAKAIND.NS</t>
+          <t>LTF.NS</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>58.20000076293945</v>
+        <v>161.5299987792969</v>
       </c>
       <c r="D37" t="n">
-        <v>57.0099983215332</v>
+        <v>159.7400054931641</v>
       </c>
       <c r="E37" t="n">
-        <v>58.75</v>
+        <v>164.1699981689453</v>
       </c>
       <c r="F37" t="n">
-        <v>57.0099983215332</v>
+        <v>159.6600036621094</v>
       </c>
       <c r="G37" t="n">
-        <v>59.47999954223633</v>
+        <v>163.5299987792969</v>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>VISAKAIND</t>
+          <t>LTF</t>
         </is>
       </c>
     </row>
@@ -1556,27 +1556,27 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>VMM.NS</t>
+          <t>LAURUSLABS.NS</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>120.7900009155273</v>
+        <v>588.7999877929688</v>
       </c>
       <c r="D38" t="n">
-        <v>118.5999984741211</v>
+        <v>578</v>
       </c>
       <c r="E38" t="n">
-        <v>121.870002746582</v>
+        <v>590</v>
       </c>
       <c r="F38" t="n">
-        <v>116.8499984741211</v>
+        <v>572.25</v>
       </c>
       <c r="G38" t="n">
-        <v>119.1900024414062</v>
+        <v>585.9500122070312</v>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>VMM</t>
+          <t>LAURUSLABS</t>
         </is>
       </c>
     </row>
@@ -1586,27 +1586,27 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>VOLTAS.BO</t>
+          <t>NTPC.NS</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>1235.75</v>
+        <v>334.75</v>
       </c>
       <c r="D39" t="n">
-        <v>1185.800048828125</v>
+        <v>334.2000122070312</v>
       </c>
       <c r="E39" t="n">
-        <v>1239.400024414062</v>
+        <v>338.75</v>
       </c>
       <c r="F39" t="n">
-        <v>1185.800048828125</v>
+        <v>330.6000061035156</v>
       </c>
       <c r="G39" t="n">
-        <v>1224.300048828125</v>
+        <v>340</v>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>VOLTAS</t>
+          <t>NTPC</t>
         </is>
       </c>
     </row>
@@ -1616,27 +1616,27 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>WABAG.NS</t>
+          <t>ONGC.NS</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>1273.199951171875</v>
+        <v>234.9600067138672</v>
       </c>
       <c r="D40" t="n">
-        <v>1250</v>
+        <v>229.1000061035156</v>
       </c>
       <c r="E40" t="n">
-        <v>1282</v>
+        <v>235.3000030517578</v>
       </c>
       <c r="F40" t="n">
-        <v>1250</v>
+        <v>228.4499969482422</v>
       </c>
       <c r="G40" t="n">
-        <v>1292.900024414062</v>
+        <v>233.2200012207031</v>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>WABAG</t>
+          <t>ONGC</t>
         </is>
       </c>
     </row>
@@ -1646,27 +1646,27 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>WIPRO.NS</t>
+          <t>PNB.NS</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>242.0099945068359</v>
+        <v>91.97000122070312</v>
       </c>
       <c r="D41" t="n">
-        <v>236.6000061035156</v>
+        <v>90</v>
       </c>
       <c r="E41" t="n">
-        <v>242.9499969482422</v>
+        <v>92.34999847412109</v>
       </c>
       <c r="F41" t="n">
-        <v>236.5</v>
+        <v>89.44999694824219</v>
       </c>
       <c r="G41" t="n">
-        <v>241.5700073242188</v>
+        <v>91.36000061035156</v>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>WIPRO</t>
+          <t>PNB</t>
         </is>
       </c>
     </row>
@@ -1676,27 +1676,27 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>YESBANK.NS</t>
+          <t>PREMIERENE.NS</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>20.02000045776367</v>
+        <v>945.6500244140625</v>
       </c>
       <c r="D42" t="n">
-        <v>17.79999923706055</v>
+        <v>922</v>
       </c>
       <c r="E42" t="n">
-        <v>20.3700008392334</v>
+        <v>954</v>
       </c>
       <c r="F42" t="n">
-        <v>17.77000045776367</v>
+        <v>917.0499877929688</v>
       </c>
       <c r="G42" t="n">
-        <v>18.22999954223633</v>
+        <v>944.7000122070312</v>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>YESBANK</t>
+          <t>PREMIERENE</t>
         </is>
       </c>
     </row>
@@ -1706,27 +1706,27 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>AWHCL.NS</t>
+          <t>RPOWER.BO</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>503.7000122070312</v>
+        <v>38.65000152587891</v>
       </c>
       <c r="D43" t="n">
-        <v>497</v>
+        <v>37.13999938964844</v>
       </c>
       <c r="E43" t="n">
-        <v>512.9500122070312</v>
+        <v>38.84999847412109</v>
       </c>
       <c r="F43" t="n">
-        <v>495.6499938964844</v>
+        <v>37</v>
       </c>
       <c r="G43" t="n">
-        <v>509.3500061035156</v>
+        <v>38.29000091552734</v>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>AWHCL</t>
+          <t>RPOWER</t>
         </is>
       </c>
     </row>
@@ -1736,27 +1736,27 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>BANKINDIA.NS</t>
+          <t>SBIN.NS</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>110.2200012207031</v>
+        <v>779.25</v>
       </c>
       <c r="D44" t="n">
-        <v>104.1999969482422</v>
+        <v>756.5</v>
       </c>
       <c r="E44" t="n">
-        <v>111.2200012207031</v>
+        <v>781.7000122070312</v>
       </c>
       <c r="F44" t="n">
-        <v>104.1999969482422</v>
+        <v>755.5</v>
       </c>
       <c r="G44" t="n">
-        <v>107.8600006103516</v>
+        <v>769</v>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>BANKINDIA</t>
+          <t>SBIN</t>
         </is>
       </c>
     </row>
@@ -1766,27 +1766,27 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>BSOFT.NS</t>
+          <t>SUVEN.NS</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>384.4500122070312</v>
+        <v>142.4499969482422</v>
       </c>
       <c r="D45" t="n">
-        <v>376.5</v>
+        <v>136.9900054931641</v>
       </c>
       <c r="E45" t="n">
-        <v>386</v>
+        <v>144.0299987792969</v>
       </c>
       <c r="F45" t="n">
-        <v>376.2999877929688</v>
+        <v>131.9900054931641</v>
       </c>
       <c r="G45" t="n">
-        <v>385.9500122070312</v>
+        <v>137.8300018310547</v>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>BSOFT</t>
+          <t>SUVEN</t>
         </is>
       </c>
     </row>
@@ -1796,27 +1796,27 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>CONCOR.NS</t>
+          <t>TATAMOTORS.NS</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>648.6500244140625</v>
+        <v>708.5</v>
       </c>
       <c r="D46" t="n">
-        <v>645.2999877929688</v>
+        <v>667.5</v>
       </c>
       <c r="E46" t="n">
-        <v>659.1500244140625</v>
+        <v>711</v>
       </c>
       <c r="F46" t="n">
-        <v>645.2999877929688</v>
+        <v>666</v>
       </c>
       <c r="G46" t="n">
-        <v>657.4000244140625</v>
+        <v>682.8499755859375</v>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>CONCOR</t>
+          <t>TATAMOTORS</t>
         </is>
       </c>
     </row>
@@ -1826,27 +1826,27 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>GAIL.NS</t>
+          <t>TECHM.NS</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>181.6000061035156</v>
+        <v>1493.699951171875</v>
       </c>
       <c r="D47" t="n">
-        <v>178.7599945068359</v>
+        <v>1480</v>
       </c>
       <c r="E47" t="n">
-        <v>182.8999938964844</v>
+        <v>1501.300048828125</v>
       </c>
       <c r="F47" t="n">
-        <v>178.6000061035156</v>
+        <v>1478.099975585938</v>
       </c>
       <c r="G47" t="n">
-        <v>184.2700042724609</v>
+        <v>1502.800048828125</v>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>GAIL</t>
+          <t>TECHM</t>
         </is>
       </c>
     </row>
@@ -1856,27 +1856,27 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>HINDUNILVR.BO</t>
+          <t>TFCILTD.BO</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>2333.949951171875</v>
+        <v>196.3000030517578</v>
       </c>
       <c r="D48" t="n">
-        <v>2324.10009765625</v>
+        <v>195</v>
       </c>
       <c r="E48" t="n">
-        <v>2340</v>
+        <v>198.8500061035156</v>
       </c>
       <c r="F48" t="n">
-        <v>2302</v>
+        <v>185</v>
       </c>
       <c r="G48" t="n">
-        <v>2355.25</v>
+        <v>198.1999969482422</v>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>HINDUNILVR</t>
+          <t>TFCILTD</t>
         </is>
       </c>
     </row>
@@ -1886,27 +1886,27 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>RELIANCE.NS</t>
+          <t>UCOBANK.BO</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>1377.199951171875</v>
+        <v>29.59000015258789</v>
       </c>
       <c r="D49" t="n">
-        <v>1385.5</v>
+        <v>29.36000061035156</v>
       </c>
       <c r="E49" t="n">
-        <v>1394.800048828125</v>
+        <v>29.89999961853027</v>
       </c>
       <c r="F49" t="n">
-        <v>1374.5</v>
+        <v>29.04999923706055</v>
       </c>
       <c r="G49" t="n">
-        <v>1407</v>
+        <v>29.98999786376953</v>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>RELIANCE</t>
+          <t>UCOBANK</t>
         </is>
       </c>
     </row>
@@ -1916,25 +1916,445 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
+          <t>VAKRANGEE.NS</t>
+        </is>
+      </c>
+      <c r="C50" t="n">
+        <v>8.840000152587891</v>
+      </c>
+      <c r="D50" t="n">
+        <v>9</v>
+      </c>
+      <c r="E50" t="n">
+        <v>9.180000305175781</v>
+      </c>
+      <c r="F50" t="n">
+        <v>8.819999694824219</v>
+      </c>
+      <c r="G50" t="n">
+        <v>9.229999542236328</v>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>VAKRANGEE</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>VISAKAIND.NS</t>
+        </is>
+      </c>
+      <c r="C51" t="n">
+        <v>58.20000076293945</v>
+      </c>
+      <c r="D51" t="n">
+        <v>57.0099983215332</v>
+      </c>
+      <c r="E51" t="n">
+        <v>58.75</v>
+      </c>
+      <c r="F51" t="n">
+        <v>57.0099983215332</v>
+      </c>
+      <c r="G51" t="n">
+        <v>59.47999954223633</v>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>VISAKAIND</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>VMM.NS</t>
+        </is>
+      </c>
+      <c r="C52" t="n">
+        <v>120.7900009155273</v>
+      </c>
+      <c r="D52" t="n">
+        <v>118.5999984741211</v>
+      </c>
+      <c r="E52" t="n">
+        <v>121.870002746582</v>
+      </c>
+      <c r="F52" t="n">
+        <v>116.8499984741211</v>
+      </c>
+      <c r="G52" t="n">
+        <v>119.1900024414062</v>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>VMM</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>VOLTAS.BO</t>
+        </is>
+      </c>
+      <c r="C53" t="n">
+        <v>1235.75</v>
+      </c>
+      <c r="D53" t="n">
+        <v>1185.800048828125</v>
+      </c>
+      <c r="E53" t="n">
+        <v>1239.400024414062</v>
+      </c>
+      <c r="F53" t="n">
+        <v>1185.800048828125</v>
+      </c>
+      <c r="G53" t="n">
+        <v>1224.300048828125</v>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>VOLTAS</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>WABAG.NS</t>
+        </is>
+      </c>
+      <c r="C54" t="n">
+        <v>1273.199951171875</v>
+      </c>
+      <c r="D54" t="n">
+        <v>1250</v>
+      </c>
+      <c r="E54" t="n">
+        <v>1282</v>
+      </c>
+      <c r="F54" t="n">
+        <v>1250</v>
+      </c>
+      <c r="G54" t="n">
+        <v>1292.900024414062</v>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>WABAG</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>WIPRO.NS</t>
+        </is>
+      </c>
+      <c r="C55" t="n">
+        <v>242.0099945068359</v>
+      </c>
+      <c r="D55" t="n">
+        <v>236.6000061035156</v>
+      </c>
+      <c r="E55" t="n">
+        <v>242.9499969482422</v>
+      </c>
+      <c r="F55" t="n">
+        <v>236.5</v>
+      </c>
+      <c r="G55" t="n">
+        <v>241.5700073242188</v>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>WIPRO</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>YESBANK.NS</t>
+        </is>
+      </c>
+      <c r="C56" t="n">
+        <v>20.02000045776367</v>
+      </c>
+      <c r="D56" t="n">
+        <v>17.79999923706055</v>
+      </c>
+      <c r="E56" t="n">
+        <v>20.3700008392334</v>
+      </c>
+      <c r="F56" t="n">
+        <v>17.77000045776367</v>
+      </c>
+      <c r="G56" t="n">
+        <v>18.22999954223633</v>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>YESBANK</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>AWHCL.NS</t>
+        </is>
+      </c>
+      <c r="C57" t="n">
+        <v>503.7000122070312</v>
+      </c>
+      <c r="D57" t="n">
+        <v>497</v>
+      </c>
+      <c r="E57" t="n">
+        <v>512.9500122070312</v>
+      </c>
+      <c r="F57" t="n">
+        <v>495.6499938964844</v>
+      </c>
+      <c r="G57" t="n">
+        <v>509.3500061035156</v>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>AWHCL</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>BANKINDIA.NS</t>
+        </is>
+      </c>
+      <c r="C58" t="n">
+        <v>110.2200012207031</v>
+      </c>
+      <c r="D58" t="n">
+        <v>104.1999969482422</v>
+      </c>
+      <c r="E58" t="n">
+        <v>111.2200012207031</v>
+      </c>
+      <c r="F58" t="n">
+        <v>104.1999969482422</v>
+      </c>
+      <c r="G58" t="n">
+        <v>107.8600006103516</v>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>BANKINDIA</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>BSOFT.NS</t>
+        </is>
+      </c>
+      <c r="C59" t="n">
+        <v>384.4500122070312</v>
+      </c>
+      <c r="D59" t="n">
+        <v>376.5</v>
+      </c>
+      <c r="E59" t="n">
+        <v>386</v>
+      </c>
+      <c r="F59" t="n">
+        <v>376.2999877929688</v>
+      </c>
+      <c r="G59" t="n">
+        <v>385.9500122070312</v>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>BSOFT</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>CONCOR.NS</t>
+        </is>
+      </c>
+      <c r="C60" t="n">
+        <v>648.6500244140625</v>
+      </c>
+      <c r="D60" t="n">
+        <v>645.2999877929688</v>
+      </c>
+      <c r="E60" t="n">
+        <v>659.1500244140625</v>
+      </c>
+      <c r="F60" t="n">
+        <v>645.2999877929688</v>
+      </c>
+      <c r="G60" t="n">
+        <v>657.4000244140625</v>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>CONCOR</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>GAIL.NS</t>
+        </is>
+      </c>
+      <c r="C61" t="n">
+        <v>181.6000061035156</v>
+      </c>
+      <c r="D61" t="n">
+        <v>178.7599945068359</v>
+      </c>
+      <c r="E61" t="n">
+        <v>182.8999938964844</v>
+      </c>
+      <c r="F61" t="n">
+        <v>178.6000061035156</v>
+      </c>
+      <c r="G61" t="n">
+        <v>184.2700042724609</v>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>GAIL</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>HINDUNILVR.BO</t>
+        </is>
+      </c>
+      <c r="C62" t="n">
+        <v>2333.949951171875</v>
+      </c>
+      <c r="D62" t="n">
+        <v>2324.10009765625</v>
+      </c>
+      <c r="E62" t="n">
+        <v>2340</v>
+      </c>
+      <c r="F62" t="n">
+        <v>2302</v>
+      </c>
+      <c r="G62" t="n">
+        <v>2355.25</v>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>HINDUNILVR</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>RELIANCE.NS</t>
+        </is>
+      </c>
+      <c r="C63" t="n">
+        <v>1377.199951171875</v>
+      </c>
+      <c r="D63" t="n">
+        <v>1385.5</v>
+      </c>
+      <c r="E63" t="n">
+        <v>1394.800048828125</v>
+      </c>
+      <c r="F63" t="n">
+        <v>1374.5</v>
+      </c>
+      <c r="G63" t="n">
+        <v>1407</v>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>RELIANCE</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
           <t>SOUTHBANK.BO</t>
         </is>
       </c>
-      <c r="C50" t="n">
+      <c r="C64" t="n">
         <v>24.34000015258789</v>
       </c>
-      <c r="D50" t="n">
+      <c r="D64" t="n">
         <v>23.79000091552734</v>
       </c>
-      <c r="E50" t="n">
+      <c r="E64" t="n">
         <v>24.43000030517578</v>
       </c>
-      <c r="F50" t="n">
+      <c r="F64" t="n">
         <v>23.79000091552734</v>
       </c>
-      <c r="G50" t="n">
+      <c r="G64" t="n">
         <v>24.20000076293945</v>
       </c>
-      <c r="H50" t="inlineStr">
+      <c r="H64" t="inlineStr">
         <is>
           <t>SOUTHBANK</t>
         </is>

</xml_diff>